<commit_message>
Små endringer tabeller og figurer
</commit_message>
<xml_diff>
--- a/Gjeldene_analyser/Analyser_p.verdi.xlsx
+++ b/Gjeldene_analyser/Analyser_p.verdi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Breili/Documents/HINN/Masteroppgave/1. NY MASTERPROSJEKT/RESULTATER/Masteroppgave/Gjeldene_analyser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510B8E85-060C-7041-AB16-FDAAF463E0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A832E25-7456-8B49-A5B2-1B5B035CB9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35260" yWindow="1640" windowWidth="28800" windowHeight="17500" xr2:uid="{CFF79CF6-E2E2-AD4F-8873-64FBE2FFBBC1}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,10 +566,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.96799999999999997</v>
+        <v>0.51649999999999996</v>
       </c>
       <c r="E3">
-        <v>1.3899999999999999E-2</v>
+        <v>0.185</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>

</xml_diff>